<commit_message>
active renseigné sur le css - test OK
</commit_message>
<xml_diff>
--- a/audit-SEO.xlsx
+++ b/audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tarik\Desktop\Formation OC\P4_Optimisez_un_site_web_existant\TarikAboulhouda_4_16122020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6282CD-C390-41E3-A444-19397F5AC8F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19CA637-72AD-4206-B101-64414C51567B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="59">
   <si>
     <t>Catégorie</t>
   </si>
@@ -529,7 +529,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -844,8 +844,8 @@
       <c r="D15" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="3" t="b">
-        <v>0</v>
+      <c r="E15" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
modification taille police + audit
</commit_message>
<xml_diff>
--- a/audit-SEO.xlsx
+++ b/audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tarik\Desktop\Formation OC\P4_Optimisez_un_site_web_existant\TarikAboulhouda_4_16122020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19CA637-72AD-4206-B101-64414C51567B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB1F19B-6AE1-4140-9927-6F2820A4C49F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="63">
   <si>
     <t>Catégorie</t>
   </si>
@@ -202,6 +202,18 @@
   </si>
   <si>
     <t xml:space="preserve">renseigner de bon attribut afin de ne pas avoir d'erreur W3C </t>
+  </si>
+  <si>
+    <t>Police de paragraphe trop petit pour mobile</t>
+  </si>
+  <si>
+    <t>Police trop petite en dessous de 12px pour mobile</t>
+  </si>
+  <si>
+    <t>Police de paragraphe passé de 11px à 12px</t>
+  </si>
+  <si>
+    <t>https://web.dev/font-size/?utm_source=lighthouse&amp;utm_medium=devtools</t>
   </si>
 </sst>
 </file>
@@ -296,7 +308,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -310,6 +322,7 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -528,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -864,23 +877,43 @@
       <c r="E16" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="F16" s="4"/>
     </row>
-    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1860,8 +1893,9 @@
     <hyperlink ref="F11" r:id="rId7" xr:uid="{C10C7352-F07C-4D59-AD25-81CB7F915A79}"/>
     <hyperlink ref="F12" r:id="rId8" xr:uid="{F96D1B43-F00D-44B3-AADA-C944D22797C2}"/>
     <hyperlink ref="F13" r:id="rId9" xr:uid="{14F3AD3C-C876-4D03-83FE-F23A69042C51}"/>
+    <hyperlink ref="F17" r:id="rId10" xr:uid="{9AB1AABC-C2BF-4345-9626-2270AF6B7B8B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId10"/>
+  <pageSetup orientation="landscape" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modif exel, presentation pptx commencé
</commit_message>
<xml_diff>
--- a/audit-SEO.xlsx
+++ b/audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tarik\Desktop\Formation OC\P4_Optimisez_un_site_web_existant\TarikAboulhouda_4_16122020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB1F19B-6AE1-4140-9927-6F2820A4C49F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD6397D-B7B4-4275-9125-EB67B82E9C13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="66">
   <si>
     <t>Catégorie</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Utilisation d'image pour des titres / citations</t>
   </si>
   <si>
-    <t>site plus volumineux et mauvais contenu SEO, probléme de d'affichange en version mobile</t>
-  </si>
-  <si>
     <t>utilisation de balide h1,h2.. Pour les titres et balise q pour les citations</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
     <t>SEO</t>
   </si>
   <si>
-    <t>aucune information donné dans la balise title améne une mauvaise SEO</t>
-  </si>
-  <si>
     <t xml:space="preserve">donner des titres cohérent à sa page web selon son contenu </t>
   </si>
   <si>
@@ -114,9 +108,6 @@
     <t>Remplir la description avec les services de l'entreprise et le contenu de la page</t>
   </si>
   <si>
-    <t>Toogle de navigation obsoléte sur la page 2</t>
-  </si>
-  <si>
     <t>mauvais fichiers css ou js renseigné dans la page 2 - une ligne en trop dans le menu déroulant</t>
   </si>
   <si>
@@ -174,9 +165,6 @@
     <t xml:space="preserve">Renseigner des mots clés en cohérence avec sa position géographique et ses services </t>
   </si>
   <si>
-    <t>Pas de titre rensigné pour la page d'acceuil et non explicite pour la page 2</t>
-  </si>
-  <si>
     <t>Trop de lien renseigné dans le footer / lien mort réseaux sociaux</t>
   </si>
   <si>
@@ -214,6 +202,27 @@
   </si>
   <si>
     <t>https://web.dev/font-size/?utm_source=lighthouse&amp;utm_medium=devtools</t>
+  </si>
+  <si>
+    <t>SEO - Performance</t>
+  </si>
+  <si>
+    <t>SEO - Accessibilité - Performance</t>
+  </si>
+  <si>
+    <t>site plus volumineux et mauvais contenu SEO, probléme de d'affichage en version mobile</t>
+  </si>
+  <si>
+    <t>Toggle de navigation obsoléte sur la page 2</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Accessibilit%C3%A9/Checklist_accessibilite_mobile</t>
+  </si>
+  <si>
+    <t>Pas de titre renseigné pour la page d'acceuil et non explicite pour la page 2</t>
+  </si>
+  <si>
+    <t>aucune information donné dans la balise title amène une mauvaise SEO</t>
   </si>
 </sst>
 </file>
@@ -542,12 +551,12 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="27.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="65.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="79.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="77.21875" bestFit="1" customWidth="1"/>
@@ -598,193 +607,193 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="E4" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="E5" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="E6" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>28</v>
-      </c>
       <c r="E7" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="E11" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -792,39 +801,39 @@
         <v>6</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -832,47 +841,50 @@
         <v>6</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E16" s="3" t="b">
         <v>0</v>
@@ -884,19 +896,19 @@
         <v>6</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1894,8 +1906,9 @@
     <hyperlink ref="F12" r:id="rId8" xr:uid="{F96D1B43-F00D-44B3-AADA-C944D22797C2}"/>
     <hyperlink ref="F13" r:id="rId9" xr:uid="{14F3AD3C-C876-4D03-83FE-F23A69042C51}"/>
     <hyperlink ref="F17" r:id="rId10" xr:uid="{9AB1AABC-C2BF-4345-9626-2270AF6B7B8B}"/>
+    <hyperlink ref="F15" r:id="rId11" xr:uid="{D9BC05AA-43A3-41FB-B4A9-88DEA2A0043F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId11"/>
+  <pageSetup orientation="landscape" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>